<commit_message>
Individual start time tests passing.
</commit_message>
<xml_diff>
--- a/src/test/resources/devils_burdens/individual_runner_start_time/leg_1/master.xlsx
+++ b/src/test/resources/devils_burdens/individual_runner_start_time/leg_1/master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gnck/Documents/Code/race-timing/src/test/resources/devils_burdens/individual_runner_start_time/leg_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EAC4D5-BD74-E94B-A0CA-05779F1E7EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A6A016-3C5A-D14A-8086-A80B8AAFD38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="2540" windowWidth="22880" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11800" yWindow="25800" windowWidth="34260" windowHeight="23080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple_detailed_2020" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Pos</t>
   </si>
@@ -179,12 +179,6 @@
     <t># recorded but the runners DNF'd the leg.</t>
   </si>
   <si>
-    <t>Recorded Split 3</t>
-  </si>
-  <si>
-    <t>Recorded Split 4</t>
-  </si>
-  <si>
     <t>Split 4</t>
   </si>
   <si>
@@ -195,6 +189,18 @@
   </si>
   <si>
     <t>INDIVIDUAL_LEG_STARTS = 2/1/0:10:00</t>
+  </si>
+  <si>
+    <t>Recorded Finish Leg 3</t>
+  </si>
+  <si>
+    <t>Recorded Finish Leg 4</t>
+  </si>
+  <si>
+    <t>Recorded Finish Leg 1</t>
+  </si>
+  <si>
+    <t>Recorded Finish Leg 2</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1079,9 +1085,10 @@
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1128,16 +1135,22 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" t="s">
         <v>48</v>
       </c>
       <c r="S1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="T1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1154,56 +1167,64 @@
         <v>17</v>
       </c>
       <c r="F2" s="1">
-        <f>G2</f>
+        <f>S2</f>
         <v>2.9664351851851855E-2</v>
       </c>
       <c r="G2" s="1">
+        <f>F2</f>
+        <v>2.9664351851851855E-2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I6" si="0">T2-S2</f>
+        <v>3.0752314814814812E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" ref="J2:J6" si="1">G2+I2</f>
+        <v>6.0416666666666667E-2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1">
+        <f>U2-MIN(L$10,T2)</f>
+        <v>4.7280092592592589E-2</v>
+      </c>
+      <c r="M2" s="1">
+        <f t="shared" ref="M2:M6" si="2">J2+L2</f>
+        <v>0.10769675925925926</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1">
+        <f>V2-MIN(O$10,U2)</f>
+        <v>5.0613425925925937E-2</v>
+      </c>
+      <c r="P2" s="1">
+        <f t="shared" ref="P2:P3" si="3">M2+O2</f>
+        <v>0.15831018518518519</v>
+      </c>
+      <c r="S2" s="1">
         <f>B16</f>
         <v>2.9664351851851855E-2</v>
       </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1">
-        <f>J2-G2</f>
-        <v>3.0752314814814812E-2</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="T2" s="1">
         <f>B17</f>
         <v>6.0416666666666667E-2</v>
       </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="1">
-        <f>R2-MIN(L$10,J2)</f>
-        <v>4.7280092592592589E-2</v>
-      </c>
-      <c r="M2" s="1">
-        <f t="shared" ref="M2:M6" si="0">J2+L2</f>
-        <v>0.10769675925925926</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="1">
-        <f>S2-MIN(O$10,R2)</f>
-        <v>5.0613425925925937E-2</v>
-      </c>
-      <c r="P2" s="1">
-        <f t="shared" ref="P2:P3" si="1">M2+O2</f>
-        <v>0.15831018518518519</v>
-      </c>
-      <c r="R2" s="1">
+      <c r="U2" s="1">
         <f>B18</f>
         <v>0.10769675925925926</v>
       </c>
-      <c r="S2" s="1">
+      <c r="V2" s="1">
         <f>B19</f>
         <v>0.15831018518518519</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1220,56 +1241,64 @@
         <v>23</v>
       </c>
       <c r="F3" s="1">
-        <f>G3</f>
+        <f>S3-G14</f>
         <v>2.3518518518518522E-2</v>
       </c>
       <c r="G3" s="1">
-        <f>B20-G14</f>
+        <f t="shared" ref="G3:G6" si="4">F3</f>
         <v>2.3518518518518522E-2</v>
       </c>
       <c r="H3" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="1">
-        <f>J3-G3</f>
-        <v>4.8101851851851854E-2</v>
+        <f>T3-S3</f>
+        <v>4.1157407407407406E-2</v>
       </c>
       <c r="J3" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4675925925925928E-2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L6" si="5">U3-MIN(L$10,T3)</f>
+        <v>3.6412037037037048E-2</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10108796296296298</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1">
+        <f>V3-MIN(O$10,U3)</f>
+        <v>5.0636574074074056E-2</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" si="3"/>
+        <v>0.15172453703703703</v>
+      </c>
+      <c r="S3" s="1">
+        <f>B20</f>
+        <v>3.0462962962962966E-2</v>
+      </c>
+      <c r="T3" s="1">
         <f>B21</f>
         <v>7.1620370370370376E-2</v>
       </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="1">
-        <f>R3-MIN(L$10,J3)</f>
-        <v>3.6412037037037048E-2</v>
-      </c>
-      <c r="M3" s="1">
-        <f t="shared" si="0"/>
-        <v>0.10803240740740742</v>
-      </c>
-      <c r="N3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="1">
-        <f>S3-MIN(O$10,R3)</f>
-        <v>5.0636574074074056E-2</v>
-      </c>
-      <c r="P3" s="1">
-        <f t="shared" si="1"/>
-        <v>0.15866898148148148</v>
-      </c>
-      <c r="R3" s="1">
+      <c r="U3" s="1">
         <f>B22</f>
         <v>0.10803240740740742</v>
       </c>
-      <c r="S3" s="1">
+      <c r="V3" s="1">
         <f>B23</f>
         <v>0.15866898148148148</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1286,29 +1315,29 @@
         <v>40</v>
       </c>
       <c r="F4" s="1">
-        <f>G4</f>
+        <f>S4</f>
         <v>3.123842592592593E-2</v>
       </c>
       <c r="G4" s="1">
-        <f>B24</f>
+        <f t="shared" si="4"/>
         <v>3.123842592592593E-2</v>
       </c>
       <c r="H4" t="s">
         <v>41</v>
       </c>
       <c r="I4" s="1">
-        <f>J4-G4</f>
+        <f t="shared" si="0"/>
         <v>4.0844907407407399E-2</v>
       </c>
       <c r="J4" s="1">
-        <f>B25</f>
+        <f t="shared" si="1"/>
         <v>7.2083333333333333E-2</v>
       </c>
       <c r="K4" t="s">
         <v>42</v>
       </c>
       <c r="L4" s="1">
-        <f>R4-MIN(L$10,J4)</f>
+        <f t="shared" si="5"/>
         <v>3.6238425925925924E-2</v>
       </c>
       <c r="M4" s="1">
@@ -1319,23 +1348,31 @@
         <v>43</v>
       </c>
       <c r="O4" s="1">
-        <f>S4-MIN(O$10,R4)</f>
+        <f>V4-MIN(O$10,U4)</f>
         <v>5.8344907407407401E-2</v>
       </c>
       <c r="P4" s="1">
         <f>M4+O4</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
+        <f>B24</f>
+        <v>3.123842592592593E-2</v>
+      </c>
+      <c r="T4" s="1">
+        <f>B25</f>
+        <v>7.2083333333333333E-2</v>
+      </c>
+      <c r="U4" s="1">
         <f>B26</f>
         <v>0.10832175925925926</v>
       </c>
-      <c r="S4" s="1">
+      <c r="V4" s="1">
         <f>B27</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1352,56 +1389,64 @@
         <v>29</v>
       </c>
       <c r="F5" s="1">
-        <f>G5</f>
+        <f t="shared" ref="F5:F6" si="6">S5</f>
         <v>3.1655092592592596E-2</v>
       </c>
       <c r="G5" s="1">
+        <f t="shared" si="4"/>
+        <v>3.1655092592592596E-2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2916666666666659E-2</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4571759259259254E-2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="5"/>
+        <v>3.3877314814814818E-2</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10844907407407407</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="1">
+        <f>V5-MIN(O$10,U5)</f>
+        <v>5.1296296296296312E-2</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" ref="P5:P6" si="7">M5+O5</f>
+        <v>0.1597453703703704</v>
+      </c>
+      <c r="S5" s="1">
         <f>B28</f>
         <v>3.1655092592592596E-2</v>
       </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="1">
-        <f>J5-G5</f>
-        <v>4.2916666666666659E-2</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="T5" s="1">
         <f>B29</f>
         <v>7.4571759259259254E-2</v>
       </c>
-      <c r="K5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="1">
-        <f>R5-MIN(L$10,J5)</f>
-        <v>3.3877314814814818E-2</v>
-      </c>
-      <c r="M5" s="1">
-        <f t="shared" si="0"/>
-        <v>0.10844907407407407</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="1">
-        <f>S5-MIN(O$10,R5)</f>
-        <v>5.1296296296296312E-2</v>
-      </c>
-      <c r="P5" s="1">
-        <f t="shared" ref="P5:P6" si="2">M5+O5</f>
-        <v>0.1597453703703704</v>
-      </c>
-      <c r="R5" s="1">
+      <c r="U5" s="1">
         <f>B30</f>
         <v>0.10844907407407407</v>
       </c>
-      <c r="S5" s="1">
+      <c r="V5" s="1">
         <f>B31</f>
         <v>0.15962962962962965</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>5</v>
       </c>
@@ -1415,68 +1460,76 @@
         <v>35</v>
       </c>
       <c r="F6" s="1">
-        <f>G6</f>
+        <f t="shared" si="6"/>
         <v>3.1747685185185184E-2</v>
       </c>
       <c r="G6" s="1">
+        <f t="shared" si="4"/>
+        <v>3.1747685185185184E-2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3067129629629636E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>7.481481481481482E-2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="5"/>
+        <v>3.4432870370370364E-2</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10924768518518518</v>
+      </c>
+      <c r="N6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="1">
+        <f>V6-MIN(O$10,U6)</f>
+        <v>5.0937499999999997E-2</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="7"/>
+        <v>0.16018518518518518</v>
+      </c>
+      <c r="S6" s="1">
         <f>B32</f>
         <v>3.1747685185185184E-2</v>
       </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="1">
-        <f>J6-G6</f>
-        <v>4.3067129629629636E-2</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="T6" s="1">
         <f>B33</f>
         <v>7.481481481481482E-2</v>
       </c>
-      <c r="K6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="1">
-        <f>R6-MIN(L$10,J6)</f>
-        <v>3.4432870370370364E-2</v>
-      </c>
-      <c r="M6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.10924768518518518</v>
-      </c>
-      <c r="N6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="1">
-        <f>S6-MIN(O$10,R6)</f>
-        <v>5.0937499999999997E-2</v>
-      </c>
-      <c r="P6" s="1">
-        <f t="shared" si="2"/>
-        <v>0.16018518518518518</v>
-      </c>
-      <c r="R6" s="1">
+      <c r="U6" s="1">
         <f>B34</f>
         <v>0.10924768518518518</v>
       </c>
-      <c r="S6" s="1">
+      <c r="V6" s="1">
         <f>B35</f>
         <v>0.15927083333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L10" s="4">
         <v>0.99998842592592585</v>
@@ -1486,7 +1539,7 @@
       </c>
       <c r="P10" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -1494,7 +1547,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -1502,12 +1555,12 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G14" s="1">
         <v>6.9444444444444441E-3</v>
@@ -1516,12 +1569,12 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="L15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>

</xml_diff>